<commit_message>
Adding Topics of Lda Model
</commit_message>
<xml_diff>
--- a/LDA_Topics.xlsx
+++ b/LDA_Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayush\Github\Uk_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qmulprod-my.sharepoint.com/personal/bsx070_qmul_ac_uk/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{339CBD19-574C-487B-B1D6-D6E6328868CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{7278E087-F6FB-4CA9-A564-A5393217E234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{16F68888-9658-4EB8-B6CD-D37CC4BBCC0D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{16F68888-9658-4EB8-B6CD-D37CC4BBCC0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Topic 0</t>
   </si>
@@ -70,6 +70,24 @@
   </si>
   <si>
     <t xml:space="preserve"> 0.017*"water" + 0.010*"power" + 0.008*"carbon" + 0.008*"photo" + 0.007*"engin" + 0.007*"product" + 0.006*"skin" + 0.005*"clean" + 0.005*"come" + 0.005*"process"</t>
+  </si>
+  <si>
+    <t>fueling electric and zero emission futuristic technology</t>
+  </si>
+  <si>
+    <t>international event/summit/confernce on renewable energy and power sources</t>
+  </si>
+  <si>
+    <t>State and government support towards climate change and clean renewable energy</t>
+  </si>
+  <si>
+    <t>Clean byproducts and low carbon outcome</t>
+  </si>
+  <si>
+    <t>Green and renewable power plant development instead of nuclear projets</t>
+  </si>
+  <si>
+    <t>Alternative fuel for NASA rocket launches and flights which creates carcinogenics</t>
   </si>
 </sst>
 </file>
@@ -429,13 +447,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3E9CA-21B6-4C22-974E-C5341903C063}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -447,6 +465,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>2</v>
@@ -457,6 +480,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>4</v>
@@ -467,6 +495,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>6</v>
@@ -477,6 +510,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>8</v>
@@ -487,6 +525,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>10</v>
@@ -495,6 +538,11 @@
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>